<commit_message>
Median work with two weeks of data
</commit_message>
<xml_diff>
--- a/Figure 11 - Median Cell Model/MD50Plot.xlsx
+++ b/Figure 11 - Median Cell Model/MD50Plot.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="14420" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="14420" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Monthly" sheetId="1" r:id="rId1"/>
+    <sheet name="2 Week" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>2008 STFZ</t>
   </si>
@@ -49,10 +50,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,13 +92,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -138,7 +167,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Monthly!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -168,7 +197,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:f>Monthly!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -195,7 +224,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:f>Monthly!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -691,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -773,6 +802,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -780,4 +810,99 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.70760000000000001</v>
+      </c>
+      <c r="C2">
+        <v>0.91500000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.65849999999999997</v>
+      </c>
+      <c r="C3">
+        <v>0.85609999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.6079</v>
+      </c>
+      <c r="C4">
+        <v>0.93069999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.34029999999999999</v>
+      </c>
+      <c r="C5">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.50360000000000005</v>
+      </c>
+      <c r="C6">
+        <v>1.1407</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0.33510000000000001</v>
+      </c>
+      <c r="C7">
+        <v>1.0886</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>